<commit_message>
Editorial correction to S-158:98 0.2.1 list of checks
</commit_message>
<xml_diff>
--- a/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
+++ b/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\S-100-Validation-Checks\Documents\S-158-98\0.2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9401B1-7954-48F4-97FB-DA525B0BB71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B9A34-DA7B-4B19-9710-49A4D933A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" activeTab="1" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" activeTab="6" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="S100ValiSpec metadata" sheetId="11" r:id="rId1"/>
@@ -3174,8 +3174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5CB01B-C150-46B9-A3FF-6538EAFBFA22}">
   <dimension ref="A1:Q453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
@@ -11607,8 +11607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F054C1B6-5AE4-4460-BB7A-387EA2B1E3C3}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11762,7 +11762,7 @@
         <v>7001</v>
       </c>
       <c r="D8">
-        <v>7009</v>
+        <v>7010</v>
       </c>
       <c r="E8" s="84">
         <v>45641</v>

</xml_diff>

<commit_message>
Editorial update to S-158:98 list metadata
</commit_message>
<xml_diff>
--- a/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
+++ b/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\S-100-Validation-Checks\Documents\S-158-98\0.2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B9A34-DA7B-4B19-9710-49A4D933A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCAB259-8819-48E2-B0F6-A39103DDE332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" activeTab="6" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="S100ValiSpec metadata" sheetId="11" r:id="rId1"/>
@@ -967,9 +967,6 @@
     <t>Last update</t>
   </si>
   <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">I have no idea what this means.
 </t>
@@ -1769,6 +1766,9 @@
   </si>
   <si>
     <t>S-102/S-101, S-104/S-101</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
   </si>
 </sst>
 </file>
@@ -2880,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5259F99A-ECF4-40F3-98D1-0270DF8F1219}">
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2959,7 +2959,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>212</v>
+        <v>302</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -2971,7 +2971,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="29">
-        <v>45627</v>
+        <v>45641</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -3242,7 +3242,7 @@
         <v>171</v>
       </c>
       <c r="N1" s="92" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O1" s="37" t="s">
         <v>28</v>
@@ -3259,10 +3259,10 @@
         <v>106</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>30</v>
@@ -3271,18 +3271,18 @@
         <v>30</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H2" s="61"/>
       <c r="I2" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J2" s="94"/>
       <c r="K2" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L2" s="33" t="s">
         <v>73</v>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
@@ -3304,10 +3304,10 @@
         <v>107</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>31</v>
@@ -3316,18 +3316,18 @@
         <v>31</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H3" s="61"/>
       <c r="I3" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J3" s="94"/>
       <c r="K3" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L3" s="33" t="s">
         <v>73</v>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="P3" s="43"/>
       <c r="Q3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
@@ -3349,10 +3349,10 @@
         <v>108</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>32</v>
@@ -3361,18 +3361,18 @@
         <v>32</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H4" s="61"/>
       <c r="I4" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J4" s="95"/>
       <c r="K4" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L4" s="46" t="s">
         <v>73</v>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="P4" s="43"/>
       <c r="Q4" s="47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -3394,10 +3394,10 @@
         <v>109</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>33</v>
@@ -3406,18 +3406,18 @@
         <v>33</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G5" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H5" s="61"/>
       <c r="I5" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J5" s="95"/>
       <c r="K5" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L5" s="46" t="s">
         <v>73</v>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="P5" s="43"/>
       <c r="Q5" s="47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
@@ -3439,10 +3439,10 @@
         <v>120</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>34</v>
@@ -3451,18 +3451,18 @@
         <v>34</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H6" s="61"/>
       <c r="I6" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J6" s="95"/>
       <c r="K6" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L6" s="46" t="s">
         <v>73</v>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="P6" s="30"/>
       <c r="Q6" s="47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
@@ -3484,10 +3484,10 @@
         <v>126</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>35</v>
@@ -3496,18 +3496,18 @@
         <v>35</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G7" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J7" s="95"/>
       <c r="K7" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L7" s="46" t="s">
         <v>74</v>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="P7" s="43"/>
       <c r="Q7" s="47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -3529,10 +3529,10 @@
         <v>127</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" s="49" t="s">
         <v>36</v>
@@ -3541,18 +3541,18 @@
         <v>36</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G8" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H8" s="61"/>
       <c r="I8" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J8" s="94"/>
       <c r="K8" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L8" s="46" t="s">
         <v>74</v>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="P8" s="54"/>
       <c r="Q8" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -3574,10 +3574,10 @@
         <v>128</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" s="49" t="s">
         <v>37</v>
@@ -3586,18 +3586,18 @@
         <v>37</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G9" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H9" s="61"/>
       <c r="I9" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J9" s="94"/>
       <c r="K9" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L9" s="46" t="s">
         <v>75</v>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="P9" s="54"/>
       <c r="Q9" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
@@ -3619,10 +3619,10 @@
         <v>129</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="44" t="s">
         <v>38</v>
@@ -3631,18 +3631,18 @@
         <v>38</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G10" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H10" s="61"/>
       <c r="I10" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J10" s="94"/>
       <c r="K10" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L10" s="46" t="s">
         <v>75</v>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="P10" s="43"/>
       <c r="Q10" s="47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="38.25" x14ac:dyDescent="0.25">
@@ -3664,10 +3664,10 @@
         <v>119</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>168</v>
@@ -3676,18 +3676,18 @@
         <v>39</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G11" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H11" s="61"/>
       <c r="I11" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J11" s="94"/>
       <c r="K11" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L11" s="46" t="s">
         <v>73</v>
@@ -3701,7 +3701,7 @@
       </c>
       <c r="P11" s="43"/>
       <c r="Q11" s="47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="153" x14ac:dyDescent="0.25">
@@ -3709,10 +3709,10 @@
         <v>121</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>92</v>
@@ -3721,18 +3721,18 @@
         <v>40</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G12" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H12" s="61"/>
       <c r="I12" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J12" s="94"/>
       <c r="K12" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L12" s="33" t="s">
         <v>75</v>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="P12" s="43"/>
       <c r="Q12" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="102.75" x14ac:dyDescent="0.25">
@@ -3754,29 +3754,29 @@
         <v>122</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G13" s="43" t="s">
         <v>87</v>
       </c>
       <c r="H13" s="61"/>
       <c r="I13" s="54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J13" s="94" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K13" s="94"/>
       <c r="L13" s="33" t="s">
@@ -3786,14 +3786,14 @@
         <v>174</v>
       </c>
       <c r="N13" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O13" s="45">
         <v>45043</v>
       </c>
       <c r="P13" s="54"/>
       <c r="Q13" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -3801,10 +3801,10 @@
         <v>123</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D14" s="44" t="s">
         <v>41</v>
@@ -3813,7 +3813,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G14" s="43" t="s">
         <v>87</v>
@@ -3822,7 +3822,7 @@
       <c r="I14" s="33"/>
       <c r="J14" s="94"/>
       <c r="K14" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L14" s="33" t="s">
         <v>75</v>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="P14" s="54"/>
       <c r="Q14" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="64.5" x14ac:dyDescent="0.25">
@@ -3844,10 +3844,10 @@
         <v>124</v>
       </c>
       <c r="B15" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D15" s="43" t="s">
         <v>93</v>
@@ -3856,7 +3856,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>87</v>
@@ -3865,7 +3865,7 @@
       <c r="I15" s="33"/>
       <c r="J15" s="94"/>
       <c r="K15" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L15" s="33" t="s">
         <v>73</v>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="P15" s="54"/>
       <c r="Q15" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
@@ -3887,10 +3887,10 @@
         <v>125</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>95</v>
@@ -3899,7 +3899,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16" s="43" t="s">
         <v>87</v>
@@ -3908,7 +3908,7 @@
       <c r="I16" s="33"/>
       <c r="J16" s="94"/>
       <c r="K16" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L16" s="33" t="s">
         <v>76</v>
@@ -3922,7 +3922,7 @@
       </c>
       <c r="P16" s="30"/>
       <c r="Q16" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="39" x14ac:dyDescent="0.25">
@@ -3930,10 +3930,10 @@
         <v>130</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D17" s="44" t="s">
         <v>44</v>
@@ -3942,7 +3942,7 @@
         <v>44</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G17" s="43" t="s">
         <v>87</v>
@@ -3951,7 +3951,7 @@
       <c r="I17" s="33"/>
       <c r="J17" s="94"/>
       <c r="K17" s="94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L17" s="33" t="s">
         <v>76</v>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="P17" s="60"/>
       <c r="Q17" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="76.5" x14ac:dyDescent="0.25">
@@ -3973,19 +3973,19 @@
         <v>131</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G18" s="43" t="s">
         <v>87</v>
@@ -3993,17 +3993,17 @@
       <c r="H18" s="61"/>
       <c r="I18" s="33"/>
       <c r="J18" s="94" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K18" s="94"/>
       <c r="L18" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M18" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N18" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O18" s="45">
         <v>45043</v>
@@ -4015,22 +4015,22 @@
     </row>
     <row r="19" spans="1:17" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D19" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="32" t="s">
         <v>245</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>259</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>246</v>
       </c>
       <c r="G19" s="43" t="s">
         <v>87</v>
@@ -4043,79 +4043,79 @@
         <v>73</v>
       </c>
       <c r="M19" s="69" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N19" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O19" s="45"/>
       <c r="P19" s="54"/>
     </row>
     <row r="20" spans="1:17" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>244</v>
-      </c>
       <c r="E20" s="36" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H20" s="61"/>
       <c r="I20" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J20" s="94"/>
       <c r="K20" s="94"/>
       <c r="L20" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M20" s="69" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N20" s="99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O20" s="45"/>
       <c r="P20" s="54"/>
     </row>
     <row r="21" spans="1:17" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="E21" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>279</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>281</v>
-      </c>
       <c r="F21" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H21" s="61"/>
       <c r="I21" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J21" s="94"/>
       <c r="K21" s="94"/>
@@ -4134,10 +4134,10 @@
         <v>132</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>94</v>
@@ -4146,7 +4146,7 @@
         <v>45</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G22" s="43" t="s">
         <v>87</v>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="P22" s="43"/>
       <c r="Q22" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -4175,10 +4175,10 @@
         <v>133</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>176</v>
@@ -4187,7 +4187,7 @@
         <v>46</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G23" s="43" t="s">
         <v>87</v>
@@ -4216,10 +4216,10 @@
         <v>134</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>177</v>
@@ -4228,7 +4228,7 @@
         <v>47</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G24" s="43" t="s">
         <v>87</v>
@@ -4257,10 +4257,10 @@
         <v>135</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>178</v>
@@ -4269,7 +4269,7 @@
         <v>48</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G25" s="43" t="s">
         <v>87</v>
@@ -4293,10 +4293,10 @@
         <v>136</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>96</v>
@@ -4305,7 +4305,7 @@
         <v>49</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G26" s="43" t="s">
         <v>87</v>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="P26" s="43"/>
       <c r="Q26" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -4334,10 +4334,10 @@
         <v>137</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>169</v>
@@ -4346,7 +4346,7 @@
         <v>50</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G27" s="43" t="s">
         <v>87</v>
@@ -4375,10 +4375,10 @@
         <v>138</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D28" s="44" t="s">
         <v>97</v>
@@ -4387,7 +4387,7 @@
         <v>51</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G28" s="43" t="s">
         <v>87</v>
@@ -4416,10 +4416,10 @@
         <v>139</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D29" s="44" t="s">
         <v>98</v>
@@ -4428,7 +4428,7 @@
         <v>52</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G29" s="43" t="s">
         <v>87</v>
@@ -4455,10 +4455,10 @@
         <v>140</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D30" s="44" t="s">
         <v>53</v>
@@ -4467,7 +4467,7 @@
         <v>53</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G30" s="43" t="s">
         <v>87</v>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="P30" s="43"/>
       <c r="Q30" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -4494,10 +4494,10 @@
         <v>141</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>94</v>
@@ -4533,10 +4533,10 @@
         <v>142</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>94</v>
@@ -4572,10 +4572,10 @@
         <v>143</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>99</v>
@@ -4584,7 +4584,7 @@
         <v>56</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G33" s="43" t="s">
         <v>87</v>
@@ -4611,10 +4611,10 @@
         <v>144</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>57</v>
@@ -4623,7 +4623,7 @@
         <v>57</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G34" s="43" t="s">
         <v>87</v>
@@ -4650,10 +4650,10 @@
         <v>145</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>58</v>
@@ -4662,7 +4662,7 @@
         <v>58</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G35" s="43" t="s">
         <v>87</v>
@@ -4689,10 +4689,10 @@
         <v>146</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D36" s="44" t="s">
         <v>59</v>
@@ -4701,7 +4701,7 @@
         <v>59</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G36" s="43" t="s">
         <v>87</v>
@@ -4728,10 +4728,10 @@
         <v>147</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D37" s="44" t="s">
         <v>60</v>
@@ -4740,7 +4740,7 @@
         <v>60</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G37" s="43" t="s">
         <v>87</v>
@@ -4767,10 +4767,10 @@
         <v>148</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D38" s="44" t="s">
         <v>61</v>
@@ -4779,7 +4779,7 @@
         <v>61</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G38" s="43" t="s">
         <v>87</v>
@@ -4806,10 +4806,10 @@
         <v>149</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D39" s="44" t="s">
         <v>62</v>
@@ -4818,7 +4818,7 @@
         <v>62</v>
       </c>
       <c r="F39" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G39" s="43" t="s">
         <v>87</v>
@@ -4845,10 +4845,10 @@
         <v>150</v>
       </c>
       <c r="B40" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D40" s="44" t="s">
         <v>63</v>
@@ -4857,7 +4857,7 @@
         <v>63</v>
       </c>
       <c r="F40" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G40" s="43" t="s">
         <v>87</v>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="P40" s="43"/>
       <c r="Q40" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
@@ -4884,10 +4884,10 @@
         <v>151</v>
       </c>
       <c r="B41" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D41" s="35" t="s">
         <v>64</v>
@@ -4896,7 +4896,7 @@
         <v>64</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G41" s="43" t="s">
         <v>87</v>
@@ -4923,10 +4923,10 @@
         <v>152</v>
       </c>
       <c r="B42" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D42" s="35" t="s">
         <v>65</v>
@@ -4935,7 +4935,7 @@
         <v>65</v>
       </c>
       <c r="F42" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G42" s="43" t="s">
         <v>87</v>
@@ -4962,10 +4962,10 @@
         <v>210</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D43" s="35" t="s">
         <v>203</v>
@@ -4977,13 +4977,13 @@
         <v>207</v>
       </c>
       <c r="G43" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H43" s="61" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I43" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L43" s="33" t="s">
         <v>73</v>
@@ -5001,10 +5001,10 @@
         <v>209</v>
       </c>
       <c r="B44" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>204</v>
@@ -5016,13 +5016,13 @@
         <v>207</v>
       </c>
       <c r="G44" s="43" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H44" s="61" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I44" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L44" s="33" t="s">
         <v>73</v>
@@ -5040,16 +5040,16 @@
         <v>153</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D45" s="35" t="s">
         <v>101</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F45" s="43" t="s">
         <v>180</v>
@@ -5060,7 +5060,7 @@
       <c r="H45" s="61"/>
       <c r="I45" s="33"/>
       <c r="J45" s="96" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L45" s="33" t="s">
         <v>82</v>
@@ -5074,34 +5074,34 @@
       </c>
       <c r="P45" s="54"/>
       <c r="Q45" s="85" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A46" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D46" s="35" t="s">
         <v>101</v>
       </c>
       <c r="E46" s="103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F46" s="43" t="s">
         <v>180</v>
       </c>
       <c r="G46" s="43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H46" s="61"/>
       <c r="I46" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L46" s="33" t="s">
         <v>82</v>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="P46" s="54"/>
       <c r="Q46" s="85" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
@@ -5123,10 +5123,10 @@
         <v>154</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D47" s="35" t="s">
         <v>100</v>
@@ -5154,7 +5154,7 @@
       </c>
       <c r="P47" s="54"/>
       <c r="Q47" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
@@ -5162,10 +5162,10 @@
         <v>155</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>102</v>
@@ -5174,7 +5174,7 @@
         <v>67</v>
       </c>
       <c r="F48" s="101" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G48" s="43" t="s">
         <v>87</v>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="P48" s="54"/>
       <c r="Q48" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -5201,10 +5201,10 @@
         <v>156</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D49" s="44" t="s">
         <v>103</v>
@@ -5232,7 +5232,7 @@
       </c>
       <c r="P49" s="54"/>
       <c r="Q49" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -5240,10 +5240,10 @@
         <v>157</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D50" s="44" t="s">
         <v>103</v>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="P50" s="54"/>
       <c r="Q50" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
@@ -5279,10 +5279,10 @@
         <v>158</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D51" s="44" t="s">
         <v>104</v>
@@ -5291,7 +5291,7 @@
         <v>70</v>
       </c>
       <c r="F51" s="102" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G51" s="43" t="s">
         <v>87</v>
@@ -5310,7 +5310,7 @@
       </c>
       <c r="P51" s="54"/>
       <c r="Q51" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -5318,19 +5318,19 @@
         <v>159</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D52" s="44" t="s">
         <v>105</v>
       </c>
       <c r="E52" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="F52" s="43" t="s">
         <v>284</v>
-      </c>
-      <c r="F52" s="43" t="s">
-        <v>285</v>
       </c>
       <c r="G52" s="43" t="s">
         <v>87</v>
@@ -5357,10 +5357,10 @@
         <v>160</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>181</v>
@@ -5388,39 +5388,39 @@
       </c>
       <c r="P53" s="43"/>
       <c r="Q53" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A54" s="106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B54" s="107" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C54" s="106" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D54" s="102" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E54" s="104" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F54" s="105" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G54" s="102" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H54" s="61"/>
       <c r="I54" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J54" s="94"/>
       <c r="K54" s="94"/>
       <c r="L54" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M54" s="41" t="s">
         <v>174</v>
@@ -5429,7 +5429,7 @@
       <c r="O54" s="45"/>
       <c r="P54" s="60"/>
       <c r="Q54" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -11464,10 +11464,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -11475,7 +11475,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11483,7 +11483,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -11491,7 +11491,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11499,7 +11499,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -11524,10 +11524,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="100" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C1" s="73" t="s">
         <v>111</v>
@@ -11541,13 +11541,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -11555,10 +11555,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -11566,10 +11566,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -11592,10 +11592,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -11607,7 +11607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F054C1B6-5AE4-4460-BB7A-387EA2B1E3C3}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -11677,7 +11677,7 @@
         <v>45641</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -11697,7 +11697,7 @@
         <v>45638</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clarifications to language of S-158:98 checks
</commit_message>
<xml_diff>
--- a/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
+++ b/Documents/S-158-98/0.2.0/S-158_98_0_2_1_20241211.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\git\S-100-Validation-Checks\Documents\S-158-98\0.2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCAB259-8819-48E2-B0F6-A39103DDE332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCF40EB-C240-4BFC-9A21-AE9DA5ABCE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28080" windowHeight="18240" activeTab="1" xr2:uid="{D500D42E-56ED-44C2-B321-3F3845968AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="S100ValiSpec metadata" sheetId="11" r:id="rId1"/>
@@ -315,7 +315,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="305">
   <si>
     <t>Classification</t>
   </si>
@@ -1461,11 +1461,6 @@
     <t>S-98</t>
   </si>
   <si>
-    <t>Cells with fill values must  intersect one of the following S-101 features in the largest scale ENC:
-(1) LandArea
-(2) UnsurveyedArea</t>
-  </si>
-  <si>
     <t>Gap in bathymetric data relative to ENC</t>
   </si>
   <si>
@@ -1645,6 +1640,17 @@
     <t>Complements Dev7001, applies to case where multiple vertical/sounding datums are used.</t>
   </si>
   <si>
+    <t>Language of description adapted to restrict it to cases where the datasets do not use multiple vertical/sounding darums.
+Check whether it should be only sounding datum for the ENC or both vertical and sounding datums.</t>
+  </si>
+  <si>
+    <t>C-12.1.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TBD
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1653,7 +1659,44 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>If an S-102 and/or S-104 dataset uses only one datum,</t>
+      <t>Delete? (1) This check would invalidate any dataset that is issued late. (2) timePoint is of type DateTime, and can't be compared only to issueDate.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refer to S-102 PT input
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Made redundant by new check for holes in S-102 (Dev7009).</t>
+    </r>
+  </si>
+  <si>
+    <t>S-102/S-101, S-104/S-101</t>
+  </si>
+  <si>
+    <t>0.2.1</t>
+  </si>
+  <si>
+    <t>If the S-102 or S-104 dataset contains features with different vertical datums, each S-102/S-104 feature must use the same vertical datum as the sounding datum of the S-101 features which intersect its domain extent polygon (allowing a 1-cell(?) margin at the D.E.P. boundary where features may overlap).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If an S-102 and/or S-104 dataset uses only one vertical datum,</t>
     </r>
     <r>
       <rPr>
@@ -1662,7 +1705,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> the Vertical Datum/Sounding Datum </t>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vertical Datum/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Sounding Datum </t>
     </r>
     <r>
       <rPr>
@@ -1691,7 +1753,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>as S-102/S-104</t>
+      <t>as the vertical datum in S-102/S-104</t>
     </r>
     <r>
       <rPr>
@@ -1723,52 +1785,16 @@
     </r>
   </si>
   <si>
-    <t>Language of description adapted to restrict it to cases where the datasets do not use multiple vertical/sounding darums.
-Check whether it should be only sounding datum for the ENC or both vertical and sounding datums.</t>
-  </si>
-  <si>
-    <t>If the S-102 or S-104 dataset contains features with different vertical datums, the domain extent polygon for each S-102/S-104 feature must have the same vertical datum as the sounding datum of the S-101 features which intersect the D.E.P. (allowing a 1-cell(?) margin at the D.E.P. boundary where features may overlap).</t>
-  </si>
-  <si>
-    <t>C-12.1.1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TBD
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delete? (1) This check would invalidate any dataset that is issued late. (2) timePoint is of type DateTime, and can't be compared only to issueDate.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Refer to S-102 PT input
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Made redundant by new check for holes in S-102 (Dev7009).</t>
-    </r>
-  </si>
-  <si>
-    <t>S-102/S-101, S-104/S-101</t>
-  </si>
-  <si>
-    <t>0.2.1</t>
+    <t>Polygons with depth attribution (S-101) are not enclosed by S-102 coverage</t>
+  </si>
+  <si>
+    <t>Cells with fill values must  intersect one of the following S-101 features in the largest scale ENC:
+(1) LandArea
+(2) UnsurveyedArea
+See Note (1) in linked table.</t>
+  </si>
+  <si>
+    <t>If the gridded dataset contains features using different vertical datums, grid cells outside the corresponding domain extent polygon are ignored when the gridded feature is checked.</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2245,7 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2505,6 +2531,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2880,7 +2909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5259F99A-ECF4-40F3-98D1-0270DF8F1219}">
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2959,7 +2988,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -3174,9 +3203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5CB01B-C150-46B9-A3FF-6538EAFBFA22}">
   <dimension ref="A1:Q453"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3262,7 +3291,7 @@
         <v>216</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>30</v>
@@ -3307,7 +3336,7 @@
         <v>216</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>31</v>
@@ -3352,7 +3381,7 @@
         <v>216</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>32</v>
@@ -3397,7 +3426,7 @@
         <v>216</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>33</v>
@@ -3442,7 +3471,7 @@
         <v>216</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>34</v>
@@ -3487,7 +3516,7 @@
         <v>216</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>35</v>
@@ -3532,7 +3561,7 @@
         <v>216</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D8" s="49" t="s">
         <v>36</v>
@@ -3577,7 +3606,7 @@
         <v>216</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" s="49" t="s">
         <v>37</v>
@@ -3622,7 +3651,7 @@
         <v>216</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D10" s="44" t="s">
         <v>38</v>
@@ -3667,7 +3696,7 @@
         <v>216</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="48" t="s">
         <v>168</v>
@@ -3712,7 +3741,7 @@
         <v>216</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>92</v>
@@ -3757,13 +3786,13 @@
         <v>216</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D13" s="43" t="s">
         <v>231</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>219</v>
@@ -3804,7 +3833,7 @@
         <v>216</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D14" s="44" t="s">
         <v>41</v>
@@ -3847,7 +3876,7 @@
         <v>216</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D15" s="43" t="s">
         <v>93</v>
@@ -3890,7 +3919,7 @@
         <v>216</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>95</v>
@@ -3933,7 +3962,7 @@
         <v>216</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D17" s="44" t="s">
         <v>44</v>
@@ -3976,7 +4005,7 @@
         <v>216</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>241</v>
@@ -4021,7 +4050,7 @@
         <v>216</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>244</v>
@@ -4059,7 +4088,7 @@
         <v>216</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D20" s="32" t="s">
         <v>243</v>
@@ -4093,19 +4122,19 @@
     </row>
     <row r="21" spans="1:17" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B21" s="33" t="s">
         <v>216</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F21" s="32" t="s">
         <v>219</v>
@@ -4137,7 +4166,7 @@
         <v>216</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>94</v>
@@ -4178,7 +4207,7 @@
         <v>216</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>176</v>
@@ -4219,7 +4248,7 @@
         <v>216</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>177</v>
@@ -4260,7 +4289,7 @@
         <v>216</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>178</v>
@@ -4296,7 +4325,7 @@
         <v>216</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D26" s="43" t="s">
         <v>96</v>
@@ -4337,7 +4366,7 @@
         <v>216</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>169</v>
@@ -4378,7 +4407,7 @@
         <v>216</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D28" s="44" t="s">
         <v>97</v>
@@ -4419,7 +4448,7 @@
         <v>216</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D29" s="44" t="s">
         <v>98</v>
@@ -4458,7 +4487,7 @@
         <v>216</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D30" s="44" t="s">
         <v>53</v>
@@ -4486,7 +4515,7 @@
       </c>
       <c r="P30" s="43"/>
       <c r="Q30" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.25">
@@ -4497,7 +4526,7 @@
         <v>216</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D31" s="43" t="s">
         <v>94</v>
@@ -4536,7 +4565,7 @@
         <v>216</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>94</v>
@@ -4575,7 +4604,7 @@
         <v>216</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>99</v>
@@ -4614,7 +4643,7 @@
         <v>216</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>57</v>
@@ -4653,7 +4682,7 @@
         <v>216</v>
       </c>
       <c r="C35" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>58</v>
@@ -4692,7 +4721,7 @@
         <v>216</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D36" s="44" t="s">
         <v>59</v>
@@ -4731,7 +4760,7 @@
         <v>216</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D37" s="44" t="s">
         <v>60</v>
@@ -4770,7 +4799,7 @@
         <v>216</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D38" s="44" t="s">
         <v>61</v>
@@ -4809,7 +4838,7 @@
         <v>216</v>
       </c>
       <c r="C39" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D39" s="44" t="s">
         <v>62</v>
@@ -4848,7 +4877,7 @@
         <v>216</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D40" s="44" t="s">
         <v>63</v>
@@ -4887,7 +4916,7 @@
         <v>216</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D41" s="35" t="s">
         <v>64</v>
@@ -4926,7 +4955,7 @@
         <v>216</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D42" s="35" t="s">
         <v>65</v>
@@ -4965,7 +4994,7 @@
         <v>216</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D43" s="35" t="s">
         <v>203</v>
@@ -4980,7 +5009,7 @@
         <v>262</v>
       </c>
       <c r="H43" s="61" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I43" s="33" t="s">
         <v>235</v>
@@ -5004,7 +5033,7 @@
         <v>216</v>
       </c>
       <c r="C44" s="42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>204</v>
@@ -5019,7 +5048,7 @@
         <v>262</v>
       </c>
       <c r="H44" s="61" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="I44" s="33" t="s">
         <v>235</v>
@@ -5043,13 +5072,13 @@
         <v>216</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D45" s="35" t="s">
         <v>101</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F45" s="43" t="s">
         <v>180</v>
@@ -5074,30 +5103,30 @@
       </c>
       <c r="P45" s="54"/>
       <c r="Q45" s="85" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A46" s="42" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B46" s="33" t="s">
         <v>216</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D46" s="35" t="s">
         <v>101</v>
       </c>
       <c r="E46" s="103" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F46" s="43" t="s">
         <v>180</v>
       </c>
       <c r="G46" s="43" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H46" s="61"/>
       <c r="I46" s="33" t="s">
@@ -5115,7 +5144,7 @@
       </c>
       <c r="P46" s="54"/>
       <c r="Q46" s="85" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="63.75" x14ac:dyDescent="0.25">
@@ -5126,7 +5155,7 @@
         <v>216</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D47" s="35" t="s">
         <v>100</v>
@@ -5154,7 +5183,7 @@
       </c>
       <c r="P47" s="54"/>
       <c r="Q47" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:17" ht="89.25" x14ac:dyDescent="0.25">
@@ -5165,7 +5194,7 @@
         <v>216</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>102</v>
@@ -5174,7 +5203,7 @@
         <v>67</v>
       </c>
       <c r="F48" s="101" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G48" s="43" t="s">
         <v>87</v>
@@ -5193,7 +5222,7 @@
       </c>
       <c r="P48" s="54"/>
       <c r="Q48" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="49" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -5204,7 +5233,7 @@
         <v>216</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D49" s="44" t="s">
         <v>103</v>
@@ -5232,7 +5261,7 @@
       </c>
       <c r="P49" s="54"/>
       <c r="Q49" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="50" spans="1:17" ht="51.75" x14ac:dyDescent="0.25">
@@ -5243,10 +5272,10 @@
         <v>216</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D50" s="44" t="s">
-        <v>103</v>
+        <v>302</v>
       </c>
       <c r="E50" s="44" t="s">
         <v>69</v>
@@ -5271,7 +5300,7 @@
       </c>
       <c r="P50" s="54"/>
       <c r="Q50" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
@@ -5282,7 +5311,7 @@
         <v>216</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D51" s="44" t="s">
         <v>104</v>
@@ -5291,7 +5320,7 @@
         <v>70</v>
       </c>
       <c r="F51" s="102" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G51" s="43" t="s">
         <v>87</v>
@@ -5310,7 +5339,7 @@
       </c>
       <c r="P51" s="54"/>
       <c r="Q51" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:17" ht="51" x14ac:dyDescent="0.25">
@@ -5321,16 +5350,16 @@
         <v>216</v>
       </c>
       <c r="C52" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D52" s="44" t="s">
         <v>105</v>
       </c>
       <c r="E52" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="F52" s="43" t="s">
         <v>283</v>
-      </c>
-      <c r="F52" s="43" t="s">
-        <v>284</v>
       </c>
       <c r="G52" s="43" t="s">
         <v>87</v>
@@ -5360,7 +5389,7 @@
         <v>216</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>181</v>
@@ -5388,24 +5417,24 @@
       </c>
       <c r="P53" s="43"/>
       <c r="Q53" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:17" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A54" s="106" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B54" s="107" t="s">
         <v>216</v>
       </c>
       <c r="C54" s="106" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D54" s="102" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E54" s="104" t="s">
-        <v>263</v>
+        <v>303</v>
       </c>
       <c r="F54" s="105" t="s">
         <v>219</v>
@@ -5420,16 +5449,18 @@
       <c r="J54" s="94"/>
       <c r="K54" s="94"/>
       <c r="L54" s="33" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="M54" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="N54" s="89"/>
+      <c r="N54" s="112" t="s">
+        <v>251</v>
+      </c>
       <c r="O54" s="45"/>
       <c r="P54" s="60"/>
       <c r="Q54" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
@@ -10629,6 +10660,7 @@
     <hyperlink ref="N19" location="OverlapNotes!A1" display="Link" xr:uid="{611E1F5F-B256-41B4-AA1C-5C83D902BB84}"/>
     <hyperlink ref="N20" location="OverlapNotes!A1" display="Link" xr:uid="{6022AC1B-71E8-4323-9FE6-4EADF678871D}"/>
     <hyperlink ref="N13" location="DataDynamicity!A1" display="Link" xr:uid="{45452DCF-0E03-4E7F-8EDF-701499FE3DC4}"/>
+    <hyperlink ref="N54" location="Datums!A1" display="Link" xr:uid="{67E4DFC2-ABF8-4F45-B762-20176EDCD000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11524,10 +11556,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="100" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="73" t="s">
         <v>111</v>
@@ -11541,13 +11573,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D2" s="72" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -11555,10 +11587,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -11566,10 +11598,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -11579,15 +11611,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A944E20B-5466-4A1E-A28C-85B214B8C7C9}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.28515625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" style="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11596,6 +11628,14 @@
       </c>
       <c r="B1" s="73" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="97">
+        <v>1</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>